<commit_message>
Add API testing with postman
Updated the documents for readme
</commit_message>
<xml_diff>
--- a/documentation/test_cases.xlsx
+++ b/documentation/test_cases.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43CC7B14-2F49-44EB-83B0-CE5BF01B25AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF3B3021-127A-4DC1-9EEE-F44258C2567B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan &amp; Summary" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="201">
   <si>
     <t>Project Name</t>
   </si>
@@ -106,36 +106,7 @@
     <t>API: Functional Testing</t>
   </si>
   <si>
-    <t>[X]</t>
-  </si>
-  <si>
-    <t>[Y]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(Example: All data retrieval (GET) passed. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>POST request failure/risk documented in Bug Report</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Aptos Narrow"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.)</t>
-    </r>
+    <t>All required endpoints were covered with positive and negative/edge cases. Data retrieval (GET/PUT) is robust, but the POST endpoint failed to enforce data validation (API-P002), highlighting a critical data integrity risk.</t>
   </si>
   <si>
     <t>Deliverable</t>
@@ -163,9 +134,6 @@
   </si>
   <si>
     <t>API Test Documentation</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
   <si>
     <t>This Workbook (Sheet 5: API Testing)</t>
@@ -959,12 +927,758 @@
   <si>
     <t>Short Analysis / Result</t>
   </si>
+  <si>
+    <t>API-G001</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Retrieve all users.</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/users</t>
+  </si>
+  <si>
+    <t>200 OK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 200. 2. Response body is an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 3. Array length is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Confirmed array structure and expected collection size.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-G002</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use an invalid/ignored query parameter (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>?limit=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Status code is 200. 2. Response body size is still 10 (confirming parameter was ignored).</t>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. API handled the unsupported parameter gracefully.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-G003</t>
+  </si>
+  <si>
+    <t>/users/1</t>
+  </si>
+  <si>
+    <t>Retrieve user with ID 1.</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/users/1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 200. 2. Response body is an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> property </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>equals 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 4. Contains </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> property.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Verified structure and correct data retrieval for a single resource.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-G004</t>
+  </si>
+  <si>
+    <t>/users/id</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Retrieve a user with a non-existent ID (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/users/999</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/users/999</t>
+  </si>
+  <si>
+    <t>404 Not Found</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 404. 2. Response body is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>empty JSON object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Confirmed API correctly returns 404 for missing resources.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-P001</t>
+  </si>
+  <si>
+    <t>/posts</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Create a new post with all mandatory fields.</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/posts</t>
+  </si>
+  <si>
+    <t>{"title": "Test Post", "body": "lorem", "userId": 1}</t>
+  </si>
+  <si>
+    <t>201 Created</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 201. 2. Response body contains a new </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 3. Returned </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>matches sent title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Data Persistence).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Resource successfully created.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-P002</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attempt to create a post with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>title field missing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>{"body": "lorem", "userId": 1}</t>
+  </si>
+  <si>
+    <r>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Standard expectation)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>not 201</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 2. If 201 is returned, assert that the returned </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> is empty/null.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FAIL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. API incorrectly returned </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>201 Created</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. This is documented as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>API Risk 001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>bug_reports.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Data Integrity Risk).</t>
+    </r>
+  </si>
+  <si>
+    <t>API-U001</t>
+  </si>
+  <si>
+    <t>/posts/1</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Update the title and body of an existing post.</t>
+  </si>
+  <si>
+    <t>https://jsonplaceholder.typicode.com/posts/1</t>
+  </si>
+  <si>
+    <t>{"id": 1, "title": "UPDATED Title", "body": "New content", "userId": 1}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 200. 2. Returned </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>matches sent updated title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 3. Returned </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> is still 1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Resource successfully updated and verified.</t>
+    </r>
+  </si>
+  <si>
+    <t>API-U002</t>
+  </si>
+  <si>
+    <t>/posts/id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Attempt to update a non-existent post (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/posts/99999</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>{"id": 99999, "title": "Test"}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Status code is 404. 2. Response body is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">empty or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF444746"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PASS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+      </rPr>
+      <t>. Confirmed API correctly handles attempts to modify a non-existent resource.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1037,21 +1751,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="12"/>
       <color rgb="FF1F1F1F"/>
       <name val="Aptos Narrow"/>
@@ -1143,6 +1842,51 @@
       <color rgb="FF1F1F1F"/>
       <name val="Google Sans Text"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444746"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444746"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF444746"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1400,17 +2144,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1433,9 +2171,69 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1445,247 +2243,205 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2884,8 +3640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE54F8A9-35DE-4C10-9626-B7D2707CD3B5}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2898,247 +3654,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="18.75">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:5" ht="60.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:5" ht="18.75">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="18.75">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="28">
         <v>45994</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="5"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="18.75">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="120" customHeight="1">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="10">
         <v>3</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="10">
         <v>1</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="148.5" customHeight="1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="10">
         <v>4</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="10">
         <v>1</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="158.25" customHeight="1">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="10">
         <v>4</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="10">
         <v>2</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="57.75" customHeight="1">
-      <c r="A12" s="42" t="s">
+    <row r="12" spans="1:5" ht="103.5" customHeight="1">
+      <c r="A12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="18">
-        <v>12</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="10">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10">
+        <v>8</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="18" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="36">
+      <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="B14" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="36">
-      <c r="A14" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="D14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" ht="54" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" ht="54" customHeight="1">
-      <c r="A15" s="43" t="s">
+      <c r="C15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="D15" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" ht="64.5" customHeight="1">
+      <c r="A16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:5" ht="64.5" customHeight="1">
-      <c r="A16" s="43" t="s">
+      <c r="D16" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="1:5" ht="42" customHeight="1">
+      <c r="A17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" ht="42" customHeight="1">
-      <c r="A17" s="43" t="s">
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="1:5" ht="41.25" customHeight="1">
+      <c r="A18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="23" t="s">
+      <c r="B18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D18" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="1:5" ht="41.25" customHeight="1">
-      <c r="A18" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{68104C1E-57CB-4D65-B1E3-5DBCB031FA4A}"/>
@@ -3171,232 +3927,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="F1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="H1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="35.25" customHeight="1">
+      <c r="A2" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="B2" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="27" t="s">
+      <c r="C2" s="43" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="35.25" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="D2" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="E2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="G2" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="H2" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="47"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" ht="249.75" customHeight="1">
+      <c r="A4" s="48"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:9" ht="36.75" customHeight="1">
+      <c r="A5" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="B5" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="C5" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="249.75" customHeight="1">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="36.75" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="F5" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="G5" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="30" t="s">
+      <c r="H5" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="39"/>
+    </row>
+    <row r="7" spans="1:9" ht="292.5" customHeight="1">
+      <c r="A7" s="48"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A8" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="B8" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="C8" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="292.5" customHeight="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="31.5" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="F8" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="G8" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="H8" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="1:9" ht="358.5" customHeight="1">
+      <c r="A10" s="48"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="39"/>
+    </row>
+    <row r="11" spans="1:9" ht="35.25" customHeight="1">
+      <c r="A11" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="B11" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="C11" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="358.5" customHeight="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="35.25" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="E11" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="F11" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="G11" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="H11" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="39"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
       <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="2"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:9" ht="195" customHeight="1">
-      <c r="A13" s="38"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="2"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="H11:H13"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="H2:H4"/>
@@ -3405,34 +4188,7 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="G8:G10"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="H11:H13"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H13">
     <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="PASS">
@@ -3459,7 +4215,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3477,291 +4233,301 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="E1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="F1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="H1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="E2" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="F2" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="G2" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="H2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="49"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="53"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:9" ht="108" customHeight="1">
+      <c r="A4" s="54"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="29.25" customHeight="1">
+      <c r="A5" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="B5" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="C5" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="53"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="60"/>
-    </row>
-    <row r="4" spans="1:9" ht="108" customHeight="1">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="67"/>
-    </row>
-    <row r="5" spans="1:9" ht="29.25" customHeight="1">
-      <c r="A5" s="46" t="s">
+      <c r="E5" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="G5" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="47" t="s">
+      <c r="H5" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="49"/>
+    </row>
+    <row r="6" spans="1:9" ht="197.25" customHeight="1">
+      <c r="A6" s="53"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" hidden="1" customHeight="1">
+      <c r="A7" s="54"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="51"/>
+    </row>
+    <row r="8" spans="1:9" ht="33.75" customHeight="1">
+      <c r="A8" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" s="47" t="s">
+      <c r="B8" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="C8" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="53"/>
-    </row>
-    <row r="6" spans="1:9" ht="197.25" customHeight="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" hidden="1" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="67"/>
-    </row>
-    <row r="8" spans="1:9" ht="33.75" customHeight="1">
-      <c r="A8" s="46" t="s">
+      <c r="D8" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="E8" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="G8" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="H8" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="49"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A9" s="53"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="100.5" customHeight="1">
+      <c r="A10" s="54"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="51"/>
+    </row>
+    <row r="11" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A11" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="47" t="s">
+      <c r="B11" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="52" t="s">
+      <c r="C11" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="53"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="60"/>
-    </row>
-    <row r="10" spans="1:9" ht="100.5" customHeight="1">
-      <c r="A10" s="61"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="67"/>
-    </row>
-    <row r="11" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A11" s="46" t="s">
+      <c r="D11" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="E11" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="F11" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="G11" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="H11" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="49"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A12" s="53"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" ht="267" customHeight="1">
+      <c r="A13" s="54"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="51"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="B14" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="C14" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="53"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="54"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="60"/>
-    </row>
-    <row r="13" spans="1:9" ht="267" customHeight="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="67"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="46" t="s">
+      <c r="D14" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="E14" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="F14" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="G14" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="71" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="52" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="53"/>
+      <c r="H14" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="49"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A15" s="54"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
     </row>
     <row r="16" spans="1:9" ht="334.5" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="G2:G4"/>
@@ -3777,26 +4543,16 @@
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H16"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H16">
     <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="PASS">
@@ -3841,207 +4597,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="E1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="F1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="H1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="196.5" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="E2" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="F2" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="G2" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="76" t="s">
+      <c r="H2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="49"/>
+    </row>
+    <row r="3" spans="1:9" ht="0.75" hidden="1" customHeight="1">
+      <c r="A3" s="90"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="91"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" ht="50.25" customHeight="1">
+      <c r="A5" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="76" t="s">
+      <c r="B5" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="C5" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="53"/>
-    </row>
-    <row r="3" spans="1:9" ht="0.75" hidden="1" customHeight="1">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="60"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="81"/>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="67"/>
-    </row>
-    <row r="5" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A5" s="74" t="s">
+      <c r="D5" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="E5" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="F5" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="G5" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="H5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="49"/>
+    </row>
+    <row r="6" spans="1:9" ht="174" customHeight="1">
+      <c r="A6" s="90"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" hidden="1">
+      <c r="A7" s="91"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="51"/>
+    </row>
+    <row r="8" spans="1:9" ht="266.25" customHeight="1">
+      <c r="A8" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="B8" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="C8" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="53"/>
-    </row>
-    <row r="6" spans="1:9" ht="174" customHeight="1">
-      <c r="A6" s="77"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9" hidden="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="67"/>
-    </row>
-    <row r="8" spans="1:9" ht="266.25" customHeight="1">
-      <c r="A8" s="89" t="s">
+      <c r="D8" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="E8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="90" t="s">
+      <c r="F8" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="90" t="s">
+      <c r="G8" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="90" t="s">
+      <c r="H8" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" ht="21" customHeight="1">
+      <c r="A9" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="F8" s="90" t="s">
+      <c r="B9" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="G8" s="96" t="s">
+      <c r="C9" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="H8" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="92"/>
-    </row>
-    <row r="9" spans="1:9" ht="21" customHeight="1">
-      <c r="A9" s="74" t="s">
+      <c r="D9" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="76" t="s">
+      <c r="E9" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="G9" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>120</v>
-      </c>
-      <c r="F9" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="53"/>
+      <c r="H9" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A10" s="77"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="60"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="1:9" ht="197.25" customHeight="1">
-      <c r="A11" s="81"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="67"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="1:9">
       <c r="G12" s="1"/>
@@ -4070,19 +4826,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D2:D4"/>
@@ -4091,12 +4845,14 @@
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="H2:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H4">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="PASS">
@@ -4143,10 +4899,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43888C7-9ECA-4EAB-89F6-67353FFF2434}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4156,50 +4912,340 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="11" max="11" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="95" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="95" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="95" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="95" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="58.5" customHeight="1">
+      <c r="A2" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="B2" s="97" t="s">
         <v>145</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C2" s="98" t="s">
         <v>146</v>
       </c>
+      <c r="D2" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="98" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="98">
+        <v>200</v>
+      </c>
+      <c r="K2" s="96" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="59.25" customHeight="1">
+      <c r="A3" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="98" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="98" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="98">
+        <v>200</v>
+      </c>
+      <c r="K3" s="96" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="58.5" customHeight="1">
+      <c r="A4" s="96" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="97" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="G4" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" s="98" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="98">
+        <v>200</v>
+      </c>
+      <c r="K4" s="96" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="49.5" customHeight="1">
+      <c r="A5" s="96" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="97" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="98" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" s="99" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="98" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="98">
+        <v>404</v>
+      </c>
+      <c r="K5" s="96" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="76.5" customHeight="1">
+      <c r="A6" s="96" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="98" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="99" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="97" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" s="97" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="98" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="98">
+        <v>201</v>
+      </c>
+      <c r="K6" s="96" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="50.25" customHeight="1">
+      <c r="A7" s="96" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="98" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="98" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="97" t="s">
+        <v>183</v>
+      </c>
+      <c r="H7" s="96" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="98" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="98">
+        <v>201</v>
+      </c>
+      <c r="K7" s="96" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="57" customHeight="1">
+      <c r="A8" s="96" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" s="97" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="98" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="98" t="s">
+        <v>193</v>
+      </c>
+      <c r="J8" s="98">
+        <v>200</v>
+      </c>
+      <c r="K8" s="96" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="62.25">
+      <c r="A9" s="96" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="98" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="98" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="99" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="97" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="I9" s="98" t="s">
+        <v>199</v>
+      </c>
+      <c r="J9" s="98">
+        <v>404</v>
+      </c>
+      <c r="K9" s="96" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{5D46908E-28B6-4928-A36C-35CB545ED84C}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{F1D910D5-AE9E-40B9-96CA-D1F663411E42}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{77E74EE7-E300-4E8C-8F79-D4FFAD540929}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{0830B6AC-1A68-4971-9388-1B44DA491C7F}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{0CFD1BBF-0952-48AF-B25D-79CAB37906AB}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{B1FB4C8A-67BA-4964-A8DA-A914DF122590}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{1126A9A3-72B6-46E0-B107-32E6B7DC9216}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{AED8FACC-6FA2-4F38-8140-EA332CC64550}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>